<commit_message>
needed Q51 for calculating the productivity and sustainability indices, but other than that converted it to ordinal as previous commit explained
</commit_message>
<xml_diff>
--- a/nepal_dataframe_FA.xlsx
+++ b/nepal_dataframe_FA.xlsx
@@ -606,7 +606,7 @@
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>Q51__How_much_land_that_is_rented_or_leased_do_you_cultivate_bigha_log__continuous</t>
+          <t>Q51__How_much_land_that_is_rented_or_leased_do_you_cultivate_bigha__ordinal</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
@@ -799,7 +799,7 @@
         <v>4.442651256490317</v>
       </c>
       <c r="AI2" t="n">
-        <v>1.386294361119891</v>
+        <v>2</v>
       </c>
       <c r="AJ2" t="n">
         <v>0.6931471805599453</v>
@@ -969,7 +969,7 @@
         <v>4.997212273764115</v>
       </c>
       <c r="AI3" t="n">
-        <v>1.09861228866811</v>
+        <v>2</v>
       </c>
       <c r="AJ3" t="n">
         <v>0.6931471805599453</v>
@@ -1139,7 +1139,7 @@
         <v>4.477336814478207</v>
       </c>
       <c r="AI4" t="n">
-        <v>1.09861228866811</v>
+        <v>2</v>
       </c>
       <c r="AJ4" t="n">
         <v>1.09861228866811</v>
@@ -1309,7 +1309,7 @@
         <v>4.653960350157523</v>
       </c>
       <c r="AI5" t="n">
-        <v>1.09861228866811</v>
+        <v>2</v>
       </c>
       <c r="AJ5" t="n">
         <v>0.6931471805599453</v>
@@ -1479,7 +1479,7 @@
         <v>4.418840607796598</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ6" t="n">
         <v>0.6931471805599453</v>
@@ -1649,7 +1649,7 @@
         <v>4.736198448394496</v>
       </c>
       <c r="AI7" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ7" t="n">
         <v>0.6931471805599453</v>
@@ -1819,7 +1819,7 @@
         <v>4.219507705176107</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ8" t="n">
         <v>1.09861228866811</v>
@@ -1989,7 +1989,7 @@
         <v>4.158883083359671</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ9" t="n">
         <v>0.6931471805599453</v>
@@ -2159,7 +2159,7 @@
         <v>4.48863636973214</v>
       </c>
       <c r="AI10" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ10" t="n">
         <v>0.6931471805599453</v>
@@ -2329,7 +2329,7 @@
         <v>4.465908118654584</v>
       </c>
       <c r="AI11" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ11" t="n">
         <v>0.6931471805599453</v>
@@ -2499,7 +2499,7 @@
         <v>4.672828834461906</v>
       </c>
       <c r="AI12" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ12" t="n">
         <v>1.09861228866811</v>
@@ -2669,7 +2669,7 @@
         <v>4.634728988229636</v>
       </c>
       <c r="AI13" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ13" t="n">
         <v>0.6931471805599453</v>
@@ -2839,7 +2839,7 @@
         <v>4.634728988229636</v>
       </c>
       <c r="AI14" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ14" t="n">
         <v>1.09861228866811</v>
@@ -3009,7 +3009,7 @@
         <v>6.470799503782602</v>
       </c>
       <c r="AI15" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ15" t="n">
         <v>0.6931471805599453</v>
@@ -3179,7 +3179,7 @@
         <v>4.499809670330265</v>
       </c>
       <c r="AI16" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ16" t="n">
         <v>0.6931471805599453</v>
@@ -3349,7 +3349,7 @@
         <v>4.605170185988092</v>
       </c>
       <c r="AI17" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ17" t="n">
         <v>1.386294361119891</v>
@@ -3519,7 +3519,7 @@
         <v>4.762173934797756</v>
       </c>
       <c r="AI18" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ18" t="n">
         <v>0.6931471805599453</v>
@@ -3689,7 +3689,7 @@
         <v>4.442651256490317</v>
       </c>
       <c r="AI19" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ19" t="n">
         <v>0.6931471805599453</v>
@@ -3859,7 +3859,7 @@
         <v>4.624972813284271</v>
       </c>
       <c r="AI20" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ20" t="n">
         <v>0.6931471805599453</v>
@@ -4029,7 +4029,7 @@
         <v>4.127134385045092</v>
       </c>
       <c r="AI21" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ21" t="n">
         <v>0.6931471805599453</v>
@@ -4199,7 +4199,7 @@
         <v>4.51085950651685</v>
       </c>
       <c r="AI22" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ22" t="n">
         <v>0.6931471805599453</v>
@@ -4369,7 +4369,7 @@
         <v>4.406719247264253</v>
       </c>
       <c r="AI23" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ23" t="n">
         <v>0.6931471805599453</v>
@@ -4539,7 +4539,7 @@
         <v>4.564348191467836</v>
       </c>
       <c r="AI24" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ24" t="n">
         <v>0.6931471805599453</v>
@@ -4709,7 +4709,7 @@
         <v>4.762173934797756</v>
       </c>
       <c r="AI25" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ25" t="n">
         <v>0.6931471805599453</v>
@@ -4879,7 +4879,7 @@
         <v>4.276666119016055</v>
       </c>
       <c r="AI26" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ26" t="n">
         <v>0.6931471805599453</v>
@@ -5049,7 +5049,7 @@
         <v>4.718498871295094</v>
       </c>
       <c r="AI27" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ27" t="n">
         <v>0.6931471805599453</v>
@@ -5219,7 +5219,7 @@
         <v>4.882801922586371</v>
       </c>
       <c r="AI28" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ28" t="n">
         <v>0.6931471805599453</v>
@@ -5389,7 +5389,7 @@
         <v>4.663439094112067</v>
       </c>
       <c r="AI29" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ29" t="n">
         <v>0.6931471805599453</v>
@@ -5559,7 +5559,7 @@
         <v>4.634728988229636</v>
       </c>
       <c r="AI30" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ30" t="n">
         <v>0.6931471805599453</v>
@@ -5729,7 +5729,7 @@
         <v>4.795790545596741</v>
       </c>
       <c r="AI31" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ31" t="n">
         <v>0.6931471805599453</v>
@@ -5899,7 +5899,7 @@
         <v>4.219507705176107</v>
       </c>
       <c r="AI32" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ32" t="n">
         <v>0.6931471805599453</v>
@@ -6069,7 +6069,7 @@
         <v>4.875197323201151</v>
       </c>
       <c r="AI33" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ33" t="n">
         <v>1.09861228866811</v>
@@ -6239,7 +6239,7 @@
         <v>4.574710978503383</v>
       </c>
       <c r="AI34" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ34" t="n">
         <v>0.6931471805599453</v>
@@ -6409,7 +6409,7 @@
         <v>4.330733340286331</v>
       </c>
       <c r="AI35" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ35" t="n">
         <v>0.6931471805599453</v>
@@ -6579,7 +6579,7 @@
         <v>4.836281906951478</v>
       </c>
       <c r="AI36" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ36" t="n">
         <v>0.6931471805599453</v>
@@ -6749,7 +6749,7 @@
         <v>4.770684624465665</v>
       </c>
       <c r="AI37" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ37" t="n">
         <v>1.09861228866811</v>
@@ -6919,7 +6919,7 @@
         <v>4.418840607796598</v>
       </c>
       <c r="AI38" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ38" t="n">
         <v>0.6931471805599453</v>
@@ -7089,7 +7089,7 @@
         <v>4.442651256490317</v>
       </c>
       <c r="AI39" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ39" t="n">
         <v>0.6931471805599453</v>
@@ -7259,7 +7259,7 @@
         <v>4.532599493153256</v>
       </c>
       <c r="AI40" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ40" t="n">
         <v>0.6931471805599453</v>
@@ -7429,7 +7429,7 @@
         <v>4.574710978503383</v>
       </c>
       <c r="AI41" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ41" t="n">
         <v>0.6931471805599453</v>
@@ -7599,7 +7599,7 @@
         <v>4.356708826689592</v>
       </c>
       <c r="AI42" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ42" t="n">
         <v>1.09861228866811</v>
@@ -7769,7 +7769,7 @@
         <v>4.634728988229636</v>
       </c>
       <c r="AI43" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ43" t="n">
         <v>1.09861228866811</v>
@@ -7939,7 +7939,7 @@
         <v>4.68213122712422</v>
       </c>
       <c r="AI44" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ44" t="n">
         <v>0.6931471805599453</v>
@@ -8109,7 +8109,7 @@
         <v>4.787491742782046</v>
       </c>
       <c r="AI45" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ45" t="n">
         <v>0.6931471805599453</v>
@@ -8279,7 +8279,7 @@
         <v>4.406719247264253</v>
       </c>
       <c r="AI46" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ46" t="n">
         <v>0.6931471805599453</v>
@@ -8449,7 +8449,7 @@
         <v>4.700480365792417</v>
       </c>
       <c r="AI47" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ47" t="n">
         <v>0.6931471805599453</v>
@@ -8619,7 +8619,7 @@
         <v>4.795790545596741</v>
       </c>
       <c r="AI48" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ48" t="n">
         <v>0.6931471805599453</v>
@@ -8789,7 +8789,7 @@
         <v>4.828313737302302</v>
       </c>
       <c r="AI49" t="n">
-        <v>0.6931471805599453</v>
+        <v>1</v>
       </c>
       <c r="AJ49" t="n">
         <v>0.6931471805599453</v>
@@ -8959,7 +8959,7 @@
         <v>4.59511985013459</v>
       </c>
       <c r="AI50" t="n">
-        <v>0.5170064828410719</v>
+        <v>1</v>
       </c>
       <c r="AJ50" t="n">
         <v>0.5170064828410719</v>
@@ -9129,7 +9129,7 @@
         <v>4.644390899141372</v>
       </c>
       <c r="AI51" t="n">
-        <v>0.5170064828410719</v>
+        <v>1</v>
       </c>
       <c r="AJ51" t="n">
         <v>0.856116008838085</v>

</xml_diff>

<commit_message>
testing mixed / spearman with global winsorization, mixed won
</commit_message>
<xml_diff>
--- a/nepal_dataframe_FA.xlsx
+++ b/nepal_dataframe_FA.xlsx
@@ -826,7 +826,7 @@
         <v>1.87022812442303</v>
       </c>
       <c r="AR2" t="n">
-        <v>2.308631377696136</v>
+        <v>2</v>
       </c>
       <c r="AS2" t="n">
         <v>0.1814890557348564</v>
@@ -966,7 +966,7 @@
         <v>43422.52065972222</v>
       </c>
       <c r="AH3" t="n">
-        <v>4.997212273764115</v>
+        <v>4.897839799950911</v>
       </c>
       <c r="AI3" t="n">
         <v>2</v>
@@ -996,7 +996,7 @@
         <v>0.455394798643756</v>
       </c>
       <c r="AR3" t="n">
-        <v>2.308631377696136</v>
+        <v>2</v>
       </c>
       <c r="AS3" t="n">
         <v>0.001932234334944216</v>
@@ -1166,7 +1166,7 @@
         <v>2.493573292379365</v>
       </c>
       <c r="AR4" t="n">
-        <v>2.308631377696136</v>
+        <v>2</v>
       </c>
       <c r="AS4" t="n">
         <v>0.2425602843292251</v>
@@ -1315,7 +1315,7 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="AK5" t="n">
-        <v>6.68586094706836</v>
+        <v>6.398594934535208</v>
       </c>
       <c r="AL5" t="n">
         <v>2.079441541679836</v>
@@ -1324,7 +1324,7 @@
         <v>2.19722457733622</v>
       </c>
       <c r="AN5" t="n">
-        <v>13.81551155796377</v>
+        <v>13.30468660086356</v>
       </c>
       <c r="AO5" t="n">
         <v>14.15198350887095</v>
@@ -1339,7 +1339,7 @@
         <v>1.732050807568877</v>
       </c>
       <c r="AS5" t="n">
-        <v>1.041714083085321</v>
+        <v>1.025823431465835</v>
       </c>
       <c r="AT5" t="n">
         <v>1.030919160914859</v>
@@ -1526,7 +1526,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1816,7 +1816,7 @@
         <v>43421.51994212963</v>
       </c>
       <c r="AH8" t="n">
-        <v>4.219507705176107</v>
+        <v>4.23245935673567</v>
       </c>
       <c r="AI8" t="n">
         <v>1</v>
@@ -1825,7 +1825,7 @@
         <v>1.09861228866811</v>
       </c>
       <c r="AK8" t="n">
-        <v>7.046499677103412</v>
+        <v>6.398594934535208</v>
       </c>
       <c r="AL8" t="n">
         <v>1.791759469228055</v>
@@ -1834,7 +1834,7 @@
         <v>1.791759469228055</v>
       </c>
       <c r="AN8" t="n">
-        <v>13.81551155796377</v>
+        <v>13.30468660086356</v>
       </c>
       <c r="AO8" t="n">
         <v>13.91082164685909</v>
@@ -1849,10 +1849,10 @@
         <v>2</v>
       </c>
       <c r="AS8" t="n">
-        <v>1.169564764465894</v>
+        <v>1.025823431465835</v>
       </c>
       <c r="AT8" t="n">
-        <v>1.194505628729953</v>
+        <v>1.136144008800468</v>
       </c>
     </row>
     <row r="9">
@@ -1986,7 +1986,7 @@
         <v>43433.55394675926</v>
       </c>
       <c r="AH9" t="n">
-        <v>4.158883083359671</v>
+        <v>4.23245935673567</v>
       </c>
       <c r="AI9" t="n">
         <v>1</v>
@@ -2007,7 +2007,7 @@
         <v>11.77529742171583</v>
       </c>
       <c r="AO9" t="n">
-        <v>12.41534077536593</v>
+        <v>12.76569129060437</v>
       </c>
       <c r="AP9" t="n">
         <v>0</v>
@@ -2076,7 +2076,7 @@
         <v>3</v>
       </c>
       <c r="P10" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Q10" t="n">
         <v>2.055555555555555</v>
@@ -2511,7 +2511,7 @@
         <v>1.945910149055313</v>
       </c>
       <c r="AM12" t="n">
-        <v>2.639057329615258</v>
+        <v>2.564949357461537</v>
       </c>
       <c r="AN12" t="n">
         <v>12.42922019683638</v>
@@ -2546,7 +2546,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -3006,7 +3006,7 @@
         <v>43415.51318287037</v>
       </c>
       <c r="AH15" t="n">
-        <v>6.470799503782602</v>
+        <v>4.897839799950911</v>
       </c>
       <c r="AI15" t="n">
         <v>1</v>
@@ -3367,7 +3367,7 @@
         <v>13.30468660086356</v>
       </c>
       <c r="AO17" t="n">
-        <v>12.41534077536593</v>
+        <v>12.76569129060437</v>
       </c>
       <c r="AP17" t="n">
         <v>2</v>
@@ -3379,7 +3379,7 @@
         <v>2</v>
       </c>
       <c r="AS17" t="n">
-        <v>1.079918546733912</v>
+        <v>1.025823431465835</v>
       </c>
       <c r="AT17" t="n">
         <v>0.8988824275220484</v>
@@ -3937,7 +3937,7 @@
         <v>1</v>
       </c>
       <c r="M21" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N21" t="n">
         <v>4</v>
@@ -3946,7 +3946,7 @@
         <v>3</v>
       </c>
       <c r="P21" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Q21" t="n">
         <v>2.470588235294118</v>
@@ -4026,7 +4026,7 @@
         <v>43441.62298611111</v>
       </c>
       <c r="AH21" t="n">
-        <v>4.127134385045092</v>
+        <v>4.23245935673567</v>
       </c>
       <c r="AI21" t="n">
         <v>1</v>
@@ -4393,7 +4393,7 @@
         <v>0</v>
       </c>
       <c r="AQ23" t="n">
-        <v>0.3515112712985166</v>
+        <v>0.3980770808024077</v>
       </c>
       <c r="AR23" t="n">
         <v>2</v>
@@ -4416,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -4465,7 +4465,7 @@
         <v>0.25</v>
       </c>
       <c r="S24" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="T24" t="inlineStr">
         <is>
@@ -5747,7 +5747,7 @@
         <v>12.25486757159303</v>
       </c>
       <c r="AO31" t="n">
-        <v>12.42922019683638</v>
+        <v>12.76569129060437</v>
       </c>
       <c r="AP31" t="n">
         <v>0</v>
@@ -5776,7 +5776,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -5896,7 +5896,7 @@
         <v>43431.48875</v>
       </c>
       <c r="AH32" t="n">
-        <v>4.219507705176107</v>
+        <v>4.23245935673567</v>
       </c>
       <c r="AI32" t="n">
         <v>1</v>
@@ -6266,7 +6266,7 @@
         <v>2.54250295676653</v>
       </c>
       <c r="AR34" t="n">
-        <v>2.23606797749979</v>
+        <v>2</v>
       </c>
       <c r="AS34" t="n">
         <v>0.1644745578455265</v>
@@ -6433,7 +6433,7 @@
         <v>2</v>
       </c>
       <c r="AQ35" t="n">
-        <v>2.875179851935822</v>
+        <v>2.870157652698332</v>
       </c>
       <c r="AR35" t="n">
         <v>2</v>
@@ -7686,7 +7686,7 @@
         <v>3</v>
       </c>
       <c r="P43" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Q43" t="n">
         <v>1.761904761904762</v>
@@ -7796,7 +7796,7 @@
         <v>1.838282568880919</v>
       </c>
       <c r="AR43" t="n">
-        <v>2.23606797749979</v>
+        <v>2</v>
       </c>
       <c r="AS43" t="n">
         <v>0.2082487469032168</v>
@@ -8697,7 +8697,7 @@
         <v>1</v>
       </c>
       <c r="M49" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N49" t="n">
         <v>4</v>
@@ -8715,7 +8715,7 @@
         <v>0.75</v>
       </c>
       <c r="S49" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T49" t="inlineStr">
         <is>
@@ -8804,10 +8804,10 @@
         <v>1.791759469228055</v>
       </c>
       <c r="AN49" t="n">
-        <v>13.99783294809122</v>
+        <v>13.30468660086356</v>
       </c>
       <c r="AO49" t="n">
-        <v>14.4916654520031</v>
+        <v>14.31628645193719</v>
       </c>
       <c r="AP49" t="n">
         <v>2</v>
@@ -8819,10 +8819,10 @@
         <v>1.414213562373095</v>
       </c>
       <c r="AS49" t="n">
-        <v>1.42849068749528</v>
+        <v>1.025823431465835</v>
       </c>
       <c r="AT49" t="n">
-        <v>1.318947029453334</v>
+        <v>1.136144008800468</v>
       </c>
     </row>
     <row r="50">
@@ -8962,7 +8962,7 @@
         <v>1</v>
       </c>
       <c r="AJ50" t="n">
-        <v>0.5170064828410719</v>
+        <v>0.6931471805599453</v>
       </c>
       <c r="AK50" t="n">
         <v>5.707110264748875</v>
@@ -9046,7 +9046,7 @@
         <v>4</v>
       </c>
       <c r="P51" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="Q51" t="n">
         <v>1.148148148148148</v>
@@ -9055,7 +9055,7 @@
         <v>0.5</v>
       </c>
       <c r="S51" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T51" t="inlineStr">
         <is>
@@ -9219,7 +9219,7 @@
         <v>47</v>
       </c>
       <c r="Q52" t="n">
-        <v>3.371648351648346</v>
+        <v>2.979999999999999</v>
       </c>
       <c r="R52" t="n">
         <v>0</v>
@@ -9314,7 +9314,7 @@
         <v>2.19722457733622</v>
       </c>
       <c r="AN52" t="n">
-        <v>0</v>
+        <v>3.503809570245734</v>
       </c>
       <c r="AO52" t="n">
         <v>13.30468660086356</v>
@@ -9329,10 +9329,10 @@
         <v>1</v>
       </c>
       <c r="AS52" t="n">
-        <v>-3.763663327076709</v>
+        <v>-2.952279807941121</v>
       </c>
       <c r="AT52" t="n">
-        <v>-1.386434771566756</v>
+        <v>-1.067611178260432</v>
       </c>
     </row>
     <row r="53">
@@ -9484,7 +9484,7 @@
         <v>2.397895272798371</v>
       </c>
       <c r="AN53" t="n">
-        <v>0</v>
+        <v>3.503809570245734</v>
       </c>
       <c r="AO53" t="n">
         <v>13.99783294809122</v>
@@ -9499,10 +9499,10 @@
         <v>1</v>
       </c>
       <c r="AS53" t="n">
-        <v>-3.758691154738659</v>
+        <v>-2.952279807941121</v>
       </c>
       <c r="AT53" t="n">
-        <v>-1.068024036732992</v>
+        <v>-1.067611178260432</v>
       </c>
     </row>
     <row r="54">
@@ -9559,7 +9559,7 @@
         <v>52</v>
       </c>
       <c r="Q54" t="n">
-        <v>3.133333333333333</v>
+        <v>2.979999999999999</v>
       </c>
       <c r="R54" t="n">
         <v>0</v>
@@ -9654,7 +9654,7 @@
         <v>2.397895272798371</v>
       </c>
       <c r="AN54" t="n">
-        <v>0</v>
+        <v>3.503809570245734</v>
       </c>
       <c r="AO54" t="n">
         <v>14.07787559166224</v>
@@ -9669,10 +9669,10 @@
         <v>1</v>
       </c>
       <c r="AS54" t="n">
-        <v>-3.758691154738659</v>
+        <v>-2.952279807941121</v>
       </c>
       <c r="AT54" t="n">
-        <v>-1.134005661755507</v>
+        <v>-1.067611178260432</v>
       </c>
     </row>
     <row r="55">
@@ -9729,13 +9729,13 @@
         <v>45</v>
       </c>
       <c r="Q55" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.8994612068965517</v>
       </c>
       <c r="R55" t="n">
         <v>0</v>
       </c>
       <c r="S55" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="T55" t="inlineStr">
         <is>
@@ -9821,7 +9821,7 @@
         <v>1.791759469228055</v>
       </c>
       <c r="AM55" t="n">
-        <v>2.70805020110221</v>
+        <v>2.564949357461537</v>
       </c>
       <c r="AN55" t="n">
         <v>9.903537551286171</v>
@@ -9842,7 +9842,7 @@
         <v>-1.102911621912203</v>
       </c>
       <c r="AT55" t="n">
-        <v>-1.379142514560761</v>
+        <v>-1.067611178260432</v>
       </c>
     </row>
     <row r="56">
@@ -10003,7 +10003,7 @@
         <v>2</v>
       </c>
       <c r="AQ56" t="n">
-        <v>2.90144003072598</v>
+        <v>2.870157652698332</v>
       </c>
       <c r="AR56" t="n">
         <v>1.414213562373095</v>
@@ -10409,7 +10409,7 @@
         <v>58</v>
       </c>
       <c r="Q59" t="n">
-        <v>3</v>
+        <v>2.979999999999999</v>
       </c>
       <c r="R59" t="n">
         <v>0.25</v>
@@ -10486,7 +10486,7 @@
         <v>43431.29625</v>
       </c>
       <c r="AH59" t="n">
-        <v>5.023880520846276</v>
+        <v>4.897839799950911</v>
       </c>
       <c r="AI59" t="n">
         <v>0</v>
@@ -11023,7 +11023,7 @@
         <v>0</v>
       </c>
       <c r="AQ62" t="n">
-        <v>2.875247517661045</v>
+        <v>2.870157652698332</v>
       </c>
       <c r="AR62" t="n">
         <v>1.414213562373095</v>
@@ -11193,7 +11193,7 @@
         <v>2</v>
       </c>
       <c r="AQ63" t="n">
-        <v>3.370684507445318</v>
+        <v>2.870157652698332</v>
       </c>
       <c r="AR63" t="n">
         <v>1.732050807568877</v>
@@ -11435,7 +11435,7 @@
         <v>0.75</v>
       </c>
       <c r="S65" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T65" t="inlineStr">
         <is>
@@ -11533,7 +11533,7 @@
         <v>2</v>
       </c>
       <c r="AQ65" t="n">
-        <v>3.442655309613876</v>
+        <v>2.870157652698332</v>
       </c>
       <c r="AR65" t="n">
         <v>2</v>
@@ -11605,7 +11605,7 @@
         <v>0.25</v>
       </c>
       <c r="S66" t="n">
-        <v>0.6600000000000001</v>
+        <v>6</v>
       </c>
       <c r="T66" t="inlineStr">
         <is>
@@ -11858,7 +11858,7 @@
         <v>5.303304908059076</v>
       </c>
       <c r="AL67" t="n">
-        <v>2.233047152659878</v>
+        <v>2.19722457733622</v>
       </c>
       <c r="AM67" t="n">
         <v>1.945910149055313</v>
@@ -11936,16 +11936,16 @@
         <v>3</v>
       </c>
       <c r="P68" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q68" t="n">
-        <v>3.153846153846154</v>
+        <v>2.979999999999999</v>
       </c>
       <c r="R68" t="n">
         <v>0.5</v>
       </c>
       <c r="S68" t="n">
-        <v>34.33999999999997</v>
+        <v>30</v>
       </c>
       <c r="T68" t="inlineStr">
         <is>
@@ -12115,7 +12115,7 @@
         <v>0.5</v>
       </c>
       <c r="S69" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T69" t="inlineStr">
         <is>
@@ -12186,7 +12186,7 @@
         <v>43461.32179398148</v>
       </c>
       <c r="AH69" t="n">
-        <v>4.219507705176107</v>
+        <v>4.23245935673567</v>
       </c>
       <c r="AI69" t="n">
         <v>0</v>
@@ -12619,7 +12619,7 @@
         <v>53</v>
       </c>
       <c r="Q72" t="n">
-        <v>3</v>
+        <v>2.979999999999999</v>
       </c>
       <c r="R72" t="n">
         <v>0.75</v>
@@ -13086,7 +13086,7 @@
         <v>1</v>
       </c>
       <c r="D75" t="n">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -13287,7 +13287,7 @@
         <v>1</v>
       </c>
       <c r="M76" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N76" t="n">
         <v>3</v>
@@ -13457,7 +13457,7 @@
         <v>1</v>
       </c>
       <c r="M77" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N77" t="n">
         <v>4</v>
@@ -13546,7 +13546,7 @@
         <v>43421.31060185185</v>
       </c>
       <c r="AH77" t="n">
-        <v>4.007333185232471</v>
+        <v>4.23245935673567</v>
       </c>
       <c r="AI77" t="n">
         <v>0</v>
@@ -13558,7 +13558,7 @@
         <v>5.860786223465865</v>
       </c>
       <c r="AL77" t="n">
-        <v>2.233047152659878</v>
+        <v>2.19722457733622</v>
       </c>
       <c r="AM77" t="n">
         <v>1.09861228866811</v>
@@ -13582,7 +13582,7 @@
         <v>0.9796891021854968</v>
       </c>
       <c r="AT77" t="n">
-        <v>1.322596814292072</v>
+        <v>1.136144008800468</v>
       </c>
     </row>
     <row r="78">
@@ -13716,7 +13716,7 @@
         <v>43423.31658564815</v>
       </c>
       <c r="AH78" t="n">
-        <v>5.010635294096256</v>
+        <v>4.897839799950911</v>
       </c>
       <c r="AI78" t="n">
         <v>0</v>
@@ -13976,7 +13976,7 @@
         <v>3</v>
       </c>
       <c r="P80" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q80" t="n">
         <v>1.875</v>
@@ -14065,7 +14065,7 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="AK80" t="n">
-        <v>6.55250788703459</v>
+        <v>6.398594934535208</v>
       </c>
       <c r="AL80" t="n">
         <v>1.945910149055313</v>
@@ -14149,7 +14149,7 @@
         <v>53</v>
       </c>
       <c r="Q81" t="n">
-        <v>0.676826503923278</v>
+        <v>0.8994612068965517</v>
       </c>
       <c r="R81" t="n">
         <v>1</v>
@@ -14235,10 +14235,10 @@
         <v>1.09861228866811</v>
       </c>
       <c r="AK81" t="n">
-        <v>6.55250788703459</v>
+        <v>6.398594934535208</v>
       </c>
       <c r="AL81" t="n">
-        <v>2.233047152659878</v>
+        <v>2.19722457733622</v>
       </c>
       <c r="AM81" t="n">
         <v>1.791759469228055</v>
@@ -14259,10 +14259,10 @@
         <v>2</v>
       </c>
       <c r="AS81" t="n">
-        <v>1.026376559469536</v>
+        <v>1.025823431465835</v>
       </c>
       <c r="AT81" t="n">
-        <v>1.236425785373032</v>
+        <v>1.136144008800468</v>
       </c>
     </row>
     <row r="82">
@@ -14307,7 +14307,7 @@
         <v>1</v>
       </c>
       <c r="M82" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N82" t="n">
         <v>3</v>
@@ -14316,7 +14316,7 @@
         <v>4</v>
       </c>
       <c r="P82" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="Q82" t="n">
         <v>2.611111111111111</v>
@@ -14405,7 +14405,7 @@
         <v>1.386294361119891</v>
       </c>
       <c r="AK82" t="n">
-        <v>7.046499677103412</v>
+        <v>6.398594934535208</v>
       </c>
       <c r="AL82" t="n">
         <v>2.079441541679836</v>
@@ -14414,7 +14414,7 @@
         <v>2.19722457733622</v>
       </c>
       <c r="AN82" t="n">
-        <v>13.99783294809122</v>
+        <v>13.30468660086356</v>
       </c>
       <c r="AO82" t="n">
         <v>14.15198350887095</v>
@@ -14423,13 +14423,13 @@
         <v>2</v>
       </c>
       <c r="AQ82" t="n">
-        <v>0.3978362327641642</v>
+        <v>0.3980770808024077</v>
       </c>
       <c r="AR82" t="n">
         <v>2</v>
       </c>
       <c r="AS82" t="n">
-        <v>1.08229026523012</v>
+        <v>1.025823431465835</v>
       </c>
       <c r="AT82" t="n">
         <v>1.027676961030374</v>
@@ -14575,16 +14575,16 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="AK83" t="n">
-        <v>3.713572066704308</v>
+        <v>3.931825632724326</v>
       </c>
       <c r="AL83" t="n">
         <v>1.6094379124341</v>
       </c>
       <c r="AM83" t="n">
-        <v>2.70805020110221</v>
+        <v>2.564949357461537</v>
       </c>
       <c r="AN83" t="n">
-        <v>0</v>
+        <v>3.503809570245734</v>
       </c>
       <c r="AO83" t="n">
         <v>14.22097633273888</v>
@@ -14599,10 +14599,10 @@
         <v>1</v>
       </c>
       <c r="AS83" t="n">
-        <v>-3.891056466195669</v>
+        <v>-2.952279807941121</v>
       </c>
       <c r="AT83" t="n">
-        <v>-1.386434771566756</v>
+        <v>-1.067611178260432</v>
       </c>
     </row>
     <row r="84">
@@ -14745,7 +14745,7 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="AK84" t="n">
-        <v>3.713572066704308</v>
+        <v>3.931825632724326</v>
       </c>
       <c r="AL84" t="n">
         <v>1.791759469228055</v>
@@ -14754,7 +14754,7 @@
         <v>2.397895272798371</v>
       </c>
       <c r="AN84" t="n">
-        <v>0</v>
+        <v>3.503809570245734</v>
       </c>
       <c r="AO84" t="n">
         <v>14.07787559166224</v>
@@ -14769,10 +14769,10 @@
         <v>1</v>
       </c>
       <c r="AS84" t="n">
-        <v>-3.752630249613468</v>
+        <v>-2.952279807941121</v>
       </c>
       <c r="AT84" t="n">
-        <v>-1.172223068895773</v>
+        <v>-1.067611178260432</v>
       </c>
     </row>
     <row r="85">
@@ -14915,7 +14915,7 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="AK85" t="n">
-        <v>3.618513213549793</v>
+        <v>3.931825632724326</v>
       </c>
       <c r="AL85" t="n">
         <v>1.6094379124341</v>
@@ -14924,7 +14924,7 @@
         <v>2.564949357461537</v>
       </c>
       <c r="AN85" t="n">
-        <v>0</v>
+        <v>3.503809570245734</v>
       </c>
       <c r="AO85" t="n">
         <v>14.07787559166224</v>
@@ -14939,10 +14939,10 @@
         <v>1</v>
       </c>
       <c r="AS85" t="n">
-        <v>-3.891056466195669</v>
+        <v>-2.952279807941121</v>
       </c>
       <c r="AT85" t="n">
-        <v>-1.165274086917855</v>
+        <v>-1.067611178260432</v>
       </c>
     </row>
     <row r="86">
@@ -15005,7 +15005,7 @@
         <v>0</v>
       </c>
       <c r="S86" t="n">
-        <v>34.33999999999997</v>
+        <v>30</v>
       </c>
       <c r="T86" t="inlineStr">
         <is>
@@ -15103,7 +15103,7 @@
         <v>0</v>
       </c>
       <c r="AQ86" t="n">
-        <v>0.3830018653917177</v>
+        <v>0.3980770808024077</v>
       </c>
       <c r="AR86" t="n">
         <v>1</v>
@@ -15756,7 +15756,7 @@
         <v>43415.43997685185</v>
       </c>
       <c r="AH90" t="n">
-        <v>7.122464801919641</v>
+        <v>4.897839799950911</v>
       </c>
       <c r="AI90" t="n">
         <v>0</v>
@@ -15783,7 +15783,7 @@
         <v>2</v>
       </c>
       <c r="AQ90" t="n">
-        <v>0.341803484516867</v>
+        <v>0.3980770808024077</v>
       </c>
       <c r="AR90" t="n">
         <v>1.732050807568877</v>
@@ -15976,7 +15976,7 @@
         <v>1</v>
       </c>
       <c r="D92" t="n">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -16146,7 +16146,7 @@
         <v>1</v>
       </c>
       <c r="D93" t="n">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -16639,7 +16639,7 @@
         <v>1.414213562373095</v>
       </c>
       <c r="AS95" t="n">
-        <v>1.147990732011338</v>
+        <v>1.025823431465835</v>
       </c>
       <c r="AT95" t="n">
         <v>-0.7893157784487906</v>
@@ -16696,10 +16696,10 @@
         <v>3</v>
       </c>
       <c r="P96" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q96" t="n">
-        <v>3.076923076923077</v>
+        <v>2.979999999999999</v>
       </c>
       <c r="R96" t="n">
         <v>0.75</v>
@@ -16996,7 +16996,7 @@
         <v>1</v>
       </c>
       <c r="D98" t="n">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -17027,7 +17027,7 @@
         <v>1</v>
       </c>
       <c r="M98" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N98" t="n">
         <v>3</v>
@@ -17152,7 +17152,7 @@
         <v>0.3601066773457784</v>
       </c>
       <c r="AT98" t="n">
-        <v>1.19687900220876</v>
+        <v>1.136144008800468</v>
       </c>
     </row>
     <row r="99">
@@ -17811,7 +17811,7 @@
         <v>2.19722457733622</v>
       </c>
       <c r="AM102" t="n">
-        <v>2.70805020110221</v>
+        <v>2.564949357461537</v>
       </c>
       <c r="AN102" t="n">
         <v>12.42922019683638</v>
@@ -17966,7 +17966,7 @@
         <v>43437.28805555555</v>
       </c>
       <c r="AH103" t="n">
-        <v>5.099866427824199</v>
+        <v>4.897839799950911</v>
       </c>
       <c r="AI103" t="n">
         <v>0</v>
@@ -17993,7 +17993,7 @@
         <v>2</v>
       </c>
       <c r="AQ103" t="n">
-        <v>2.870941912841384</v>
+        <v>2.870157652698332</v>
       </c>
       <c r="AR103" t="n">
         <v>1.414213562373095</v>
@@ -18306,7 +18306,7 @@
         <v>43451.60998842592</v>
       </c>
       <c r="AH105" t="n">
-        <v>4.189654742026425</v>
+        <v>4.23245935673567</v>
       </c>
       <c r="AI105" t="n">
         <v>0</v>
@@ -18356,7 +18356,7 @@
         <v>0</v>
       </c>
       <c r="D106" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -18399,7 +18399,7 @@
         <v>45</v>
       </c>
       <c r="Q106" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8994612068965517</v>
       </c>
       <c r="R106" t="n">
         <v>0.25</v>
@@ -18526,7 +18526,7 @@
         <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -18679,10 +18679,10 @@
         <v>1.414213562373095</v>
       </c>
       <c r="AS107" t="n">
-        <v>1.432778152223154</v>
+        <v>1.025823431465835</v>
       </c>
       <c r="AT107" t="n">
-        <v>1.18168950521682</v>
+        <v>1.136144008800468</v>
       </c>
     </row>
     <row r="108">
@@ -18739,7 +18739,7 @@
         <v>54</v>
       </c>
       <c r="Q108" t="n">
-        <v>0.896551724137931</v>
+        <v>0.8994612068965517</v>
       </c>
       <c r="R108" t="n">
         <v>1</v>
@@ -18906,16 +18906,16 @@
         <v>4</v>
       </c>
       <c r="P109" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q109" t="n">
-        <v>0.676826503923278</v>
+        <v>0.8994612068965517</v>
       </c>
       <c r="R109" t="n">
         <v>0.75</v>
       </c>
       <c r="S109" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T109" t="inlineStr">
         <is>
@@ -19007,7 +19007,7 @@
         <v>12.89922232608699</v>
       </c>
       <c r="AO109" t="n">
-        <v>14.40329777842179</v>
+        <v>14.31628645193719</v>
       </c>
       <c r="AP109" t="n">
         <v>2</v>
@@ -19183,7 +19183,7 @@
         <v>2</v>
       </c>
       <c r="AQ110" t="n">
-        <v>0.37463105855764</v>
+        <v>0.3980770808024077</v>
       </c>
       <c r="AR110" t="n">
         <v>1.732050807568877</v>
@@ -19517,7 +19517,7 @@
         <v>12.89922232608699</v>
       </c>
       <c r="AO112" t="n">
-        <v>14.40329777842179</v>
+        <v>14.31628645193719</v>
       </c>
       <c r="AP112" t="n">
         <v>2</v>
@@ -19586,7 +19586,7 @@
         <v>3</v>
       </c>
       <c r="P113" t="n">
-        <v>60.33999999999997</v>
+        <v>58</v>
       </c>
       <c r="Q113" t="n">
         <v>2.578947368421053</v>
@@ -19675,7 +19675,7 @@
         <v>1.386294361119891</v>
       </c>
       <c r="AK113" t="n">
-        <v>6.55250788703459</v>
+        <v>6.398594934535208</v>
       </c>
       <c r="AL113" t="n">
         <v>1.945910149055313</v>
@@ -19684,10 +19684,10 @@
         <v>2.564949357461537</v>
       </c>
       <c r="AN113" t="n">
-        <v>13.45883704259595</v>
+        <v>13.30468660086356</v>
       </c>
       <c r="AO113" t="n">
-        <v>14.5086582385241</v>
+        <v>14.31628645193719</v>
       </c>
       <c r="AP113" t="n">
         <v>0</v>
@@ -19702,7 +19702,7 @@
         <v>-0.1006624618345745</v>
       </c>
       <c r="AT113" t="n">
-        <v>1.300720308911306</v>
+        <v>1.136144008800468</v>
       </c>
     </row>
     <row r="114">
@@ -19854,7 +19854,7 @@
         <v>1.791759469228055</v>
       </c>
       <c r="AN114" t="n">
-        <v>13.59236825664928</v>
+        <v>13.30468660086356</v>
       </c>
       <c r="AO114" t="n">
         <v>14.28551481220982</v>
@@ -20015,7 +20015,7 @@
         <v>1.386294361119891</v>
       </c>
       <c r="AK115" t="n">
-        <v>6.90875477931522</v>
+        <v>6.398594934535208</v>
       </c>
       <c r="AL115" t="n">
         <v>1.945910149055313</v>
@@ -20024,7 +20024,7 @@
         <v>2.397895272798371</v>
       </c>
       <c r="AN115" t="n">
-        <v>13.59236825664928</v>
+        <v>13.30468660086356</v>
       </c>
       <c r="AO115" t="n">
         <v>14.28551481220982</v>
@@ -20039,10 +20039,10 @@
         <v>2</v>
       </c>
       <c r="AS115" t="n">
-        <v>1.038149308017854</v>
+        <v>1.025823431465835</v>
       </c>
       <c r="AT115" t="n">
-        <v>1.198990171065268</v>
+        <v>1.136144008800468</v>
       </c>
     </row>
     <row r="116">
@@ -20099,7 +20099,7 @@
         <v>57</v>
       </c>
       <c r="Q116" t="n">
-        <v>3.285714285714286</v>
+        <v>2.979999999999999</v>
       </c>
       <c r="R116" t="n">
         <v>0.75</v>
@@ -20185,7 +20185,7 @@
         <v>1.386294361119891</v>
       </c>
       <c r="AK116" t="n">
-        <v>7.046499677103412</v>
+        <v>6.398594934535208</v>
       </c>
       <c r="AL116" t="n">
         <v>2.079441541679836</v>
@@ -20194,10 +20194,10 @@
         <v>2.564949357461537</v>
       </c>
       <c r="AN116" t="n">
-        <v>13.99783294809122</v>
+        <v>13.30468660086356</v>
       </c>
       <c r="AO116" t="n">
-        <v>14.5086582385241</v>
+        <v>14.31628645193719</v>
       </c>
       <c r="AP116" t="n">
         <v>2</v>
@@ -20209,10 +20209,10 @@
         <v>2</v>
       </c>
       <c r="AS116" t="n">
-        <v>1.432778152223154</v>
+        <v>1.025823431465835</v>
       </c>
       <c r="AT116" t="n">
-        <v>1.322596814292072</v>
+        <v>1.136144008800468</v>
       </c>
     </row>
     <row r="117">
@@ -20269,7 +20269,7 @@
         <v>52</v>
       </c>
       <c r="Q117" t="n">
-        <v>0.7428571428571429</v>
+        <v>0.8994612068965517</v>
       </c>
       <c r="R117" t="n">
         <v>0</v>
@@ -20355,7 +20355,7 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="AK117" t="n">
-        <v>3.713572066704308</v>
+        <v>3.931825632724326</v>
       </c>
       <c r="AL117" t="n">
         <v>1.6094379124341</v>
@@ -20364,7 +20364,7 @@
         <v>2.564949357461537</v>
       </c>
       <c r="AN117" t="n">
-        <v>0</v>
+        <v>3.503809570245734</v>
       </c>
       <c r="AO117" t="n">
         <v>13.99783294809122</v>
@@ -20379,10 +20379,10 @@
         <v>1</v>
       </c>
       <c r="AS117" t="n">
-        <v>-3.752630249613468</v>
+        <v>-2.952279807941121</v>
       </c>
       <c r="AT117" t="n">
-        <v>-1.079647012993119</v>
+        <v>-1.067611178260432</v>
       </c>
     </row>
     <row r="118">
@@ -20445,7 +20445,7 @@
         <v>0.25</v>
       </c>
       <c r="S118" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T118" t="inlineStr">
         <is>
@@ -21076,7 +21076,7 @@
         <v>0</v>
       </c>
       <c r="D122" t="n">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -21733,7 +21733,7 @@
         <v>2</v>
       </c>
       <c r="AQ125" t="n">
-        <v>0.3357592089059304</v>
+        <v>0.3980770808024077</v>
       </c>
       <c r="AR125" t="n">
         <v>1.414213562373095</v>
@@ -21897,7 +21897,7 @@
         <v>12.42922019683638</v>
       </c>
       <c r="AO126" t="n">
-        <v>14.40329777842179</v>
+        <v>14.31628645193719</v>
       </c>
       <c r="AP126" t="n">
         <v>2</v>
@@ -22237,7 +22237,7 @@
         <v>12.10071768541247</v>
       </c>
       <c r="AO128" t="n">
-        <v>12.73670383776449</v>
+        <v>12.76569129060437</v>
       </c>
       <c r="AP128" t="n">
         <v>0</v>
@@ -22309,7 +22309,7 @@
         <v>46</v>
       </c>
       <c r="Q129" t="n">
-        <v>3.266666666666667</v>
+        <v>2.979999999999999</v>
       </c>
       <c r="R129" t="n">
         <v>0.25</v>
@@ -22905,7 +22905,7 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="AK132" t="n">
-        <v>3.618513213549793</v>
+        <v>3.931825632724326</v>
       </c>
       <c r="AL132" t="n">
         <v>1.6094379124341</v>
@@ -22914,7 +22914,7 @@
         <v>2.397895272798371</v>
       </c>
       <c r="AN132" t="n">
-        <v>0</v>
+        <v>3.503809570245734</v>
       </c>
       <c r="AO132" t="n">
         <v>13.99783294809122</v>
@@ -22929,10 +22929,10 @@
         <v>1</v>
       </c>
       <c r="AS132" t="n">
-        <v>-3.744866173382089</v>
+        <v>-2.952279807941121</v>
       </c>
       <c r="AT132" t="n">
-        <v>-1.233716910409419</v>
+        <v>-1.067611178260432</v>
       </c>
     </row>
     <row r="133">
@@ -22995,7 +22995,7 @@
         <v>0</v>
       </c>
       <c r="S133" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T133" t="inlineStr">
         <is>
@@ -23102,7 +23102,7 @@
         <v>-1.102911621912203</v>
       </c>
       <c r="AT133" t="n">
-        <v>-1.192218636040171</v>
+        <v>-1.067611178260432</v>
       </c>
     </row>
     <row r="134">
@@ -23116,7 +23116,7 @@
         <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -23326,7 +23326,7 @@
         <v>3</v>
       </c>
       <c r="P135" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="Q135" t="n">
         <v>2.529411764705882</v>
@@ -23796,7 +23796,7 @@
         <v>0</v>
       </c>
       <c r="D138" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -24629,7 +24629,7 @@
         <v>1.414213562373095</v>
       </c>
       <c r="AS142" t="n">
-        <v>1.329951690003587</v>
+        <v>1.025823431465835</v>
       </c>
       <c r="AT142" t="n">
         <v>0.1055606943127869</v>
@@ -24816,7 +24816,7 @@
         <v>1</v>
       </c>
       <c r="D144" t="n">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -24859,13 +24859,13 @@
         <v>54</v>
       </c>
       <c r="Q144" t="n">
-        <v>0.7666666666666667</v>
+        <v>0.8994612068965517</v>
       </c>
       <c r="R144" t="n">
         <v>0.5</v>
       </c>
       <c r="S144" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="T144" t="inlineStr">
         <is>
@@ -24972,7 +24972,7 @@
         <v>-0.01878699437893509</v>
       </c>
       <c r="AT144" t="n">
-        <v>1.215981645831421</v>
+        <v>1.136144008800468</v>
       </c>
     </row>
     <row r="145">
@@ -25029,13 +25029,13 @@
         <v>53</v>
       </c>
       <c r="Q145" t="n">
-        <v>0.676826503923278</v>
+        <v>0.8994612068965517</v>
       </c>
       <c r="R145" t="n">
         <v>0.75</v>
       </c>
       <c r="S145" t="n">
-        <v>0.6600000000000001</v>
+        <v>6</v>
       </c>
       <c r="T145" t="inlineStr">
         <is>
@@ -25106,7 +25106,7 @@
         <v>43464.30665509259</v>
       </c>
       <c r="AH145" t="n">
-        <v>3.714810443399589</v>
+        <v>4.23245935673567</v>
       </c>
       <c r="AI145" t="n">
         <v>0</v>
@@ -25127,7 +25127,7 @@
         <v>13.12236537740233</v>
       </c>
       <c r="AO145" t="n">
-        <v>14.5086582385241</v>
+        <v>14.31628645193719</v>
       </c>
       <c r="AP145" t="n">
         <v>2</v>
@@ -25285,7 +25285,7 @@
         <v>1.386294361119891</v>
       </c>
       <c r="AK146" t="n">
-        <v>6.68586094706836</v>
+        <v>6.398594934535208</v>
       </c>
       <c r="AL146" t="n">
         <v>2.19722457733622</v>
@@ -25312,7 +25312,7 @@
         <v>1.012258325806236</v>
       </c>
       <c r="AT146" t="n">
-        <v>1.23040991918235</v>
+        <v>1.136144008800468</v>
       </c>
     </row>
     <row r="147">
@@ -25643,7 +25643,7 @@
         <v>0</v>
       </c>
       <c r="AQ148" t="n">
-        <v>2.873488247396438</v>
+        <v>2.870157652698332</v>
       </c>
       <c r="AR148" t="n">
         <v>1.414213562373095</v>
@@ -25965,7 +25965,7 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="AK150" t="n">
-        <v>6.478509642208569</v>
+        <v>6.398594934535208</v>
       </c>
       <c r="AL150" t="n">
         <v>1.791759469228055</v>
@@ -26006,7 +26006,7 @@
         <v>0</v>
       </c>
       <c r="D151" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -26037,7 +26037,7 @@
         <v>0</v>
       </c>
       <c r="M151" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N151" t="n">
         <v>2</v>
@@ -26046,7 +26046,7 @@
         <v>2</v>
       </c>
       <c r="P151" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q151" t="n">
         <v>1.130434782608696</v>
@@ -26144,7 +26144,7 @@
         <v>1.791759469228055</v>
       </c>
       <c r="AN151" t="n">
-        <v>0</v>
+        <v>3.503809570245734</v>
       </c>
       <c r="AO151" t="n">
         <v>14.22097633273888</v>
@@ -26159,7 +26159,7 @@
         <v>1</v>
       </c>
       <c r="AS151" t="n">
-        <v>-3.758691154738659</v>
+        <v>-2.952279807941121</v>
       </c>
       <c r="AT151" t="n">
         <v>-0.9460055359306223</v>
@@ -26225,7 +26225,7 @@
         <v>0</v>
       </c>
       <c r="S152" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T152" t="inlineStr">
         <is>
@@ -26305,7 +26305,7 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="AK152" t="n">
-        <v>3.618513213549793</v>
+        <v>3.931825632724326</v>
       </c>
       <c r="AL152" t="n">
         <v>1.6094379124341</v>
@@ -26314,7 +26314,7 @@
         <v>2.564949357461537</v>
       </c>
       <c r="AN152" t="n">
-        <v>0</v>
+        <v>3.503809570245734</v>
       </c>
       <c r="AO152" t="n">
         <v>13.99783294809122</v>
@@ -26329,7 +26329,7 @@
         <v>1</v>
       </c>
       <c r="AS152" t="n">
-        <v>-3.744866173382089</v>
+        <v>-2.952279807941121</v>
       </c>
       <c r="AT152" t="n">
         <v>-0.9546954154905245</v>
@@ -26475,7 +26475,7 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="AK153" t="n">
-        <v>3.713572066704308</v>
+        <v>3.931825632724326</v>
       </c>
       <c r="AL153" t="n">
         <v>1.791759469228055</v>
@@ -26484,7 +26484,7 @@
         <v>2.564949357461537</v>
       </c>
       <c r="AN153" t="n">
-        <v>0</v>
+        <v>3.503809570245734</v>
       </c>
       <c r="AO153" t="n">
         <v>14.15198350887095</v>
@@ -26499,7 +26499,7 @@
         <v>1</v>
       </c>
       <c r="AS153" t="n">
-        <v>-3.752630249613468</v>
+        <v>-2.952279807941121</v>
       </c>
       <c r="AT153" t="n">
         <v>-0.9226966461356356</v>
@@ -26654,7 +26654,7 @@
         <v>2.564949357461537</v>
       </c>
       <c r="AN154" t="n">
-        <v>0</v>
+        <v>3.503809570245734</v>
       </c>
       <c r="AO154" t="n">
         <v>14.03865490927816</v>
@@ -26669,7 +26669,7 @@
         <v>1</v>
       </c>
       <c r="AS154" t="n">
-        <v>-3.758691154738659</v>
+        <v>-2.952279807941121</v>
       </c>
       <c r="AT154" t="n">
         <v>-0.9117793071998089</v>
@@ -26824,7 +26824,7 @@
         <v>2.564949357461537</v>
       </c>
       <c r="AN155" t="n">
-        <v>0</v>
+        <v>3.503809570245734</v>
       </c>
       <c r="AO155" t="n">
         <v>14.22097633273888</v>
@@ -26839,7 +26839,7 @@
         <v>1</v>
       </c>
       <c r="AS155" t="n">
-        <v>-3.758691154738659</v>
+        <v>-2.952279807941121</v>
       </c>
       <c r="AT155" t="n">
         <v>-0.06035644203167396</v>
@@ -26985,7 +26985,7 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="AK156" t="n">
-        <v>6.68586094706836</v>
+        <v>6.398594934535208</v>
       </c>
       <c r="AL156" t="n">
         <v>1.945910149055313</v>
@@ -26994,7 +26994,7 @@
         <v>2.397895272798371</v>
       </c>
       <c r="AN156" t="n">
-        <v>2.19722457733622</v>
+        <v>3.503809570245734</v>
       </c>
       <c r="AO156" t="n">
         <v>13.52782981884494</v>
@@ -27009,7 +27009,7 @@
         <v>1.414213562373095</v>
       </c>
       <c r="AS156" t="n">
-        <v>-3.891056466195669</v>
+        <v>-2.952279807941121</v>
       </c>
       <c r="AT156" t="n">
         <v>0.445281846747014</v>
@@ -27155,7 +27155,7 @@
         <v>1.386294361119891</v>
       </c>
       <c r="AK157" t="n">
-        <v>6.55250788703459</v>
+        <v>6.398594934535208</v>
       </c>
       <c r="AL157" t="n">
         <v>2.079441541679836</v>
@@ -27179,7 +27179,7 @@
         <v>1.732050807568877</v>
       </c>
       <c r="AS157" t="n">
-        <v>1.377759661356759</v>
+        <v>1.025823431465835</v>
       </c>
       <c r="AT157" t="n">
         <v>-0.8132609611321915</v>
@@ -27239,7 +27239,7 @@
         <v>54</v>
       </c>
       <c r="Q158" t="n">
-        <v>0.7096774193548387</v>
+        <v>0.8994612068965517</v>
       </c>
       <c r="R158" t="n">
         <v>0.5</v>
@@ -27409,13 +27409,13 @@
         <v>53</v>
       </c>
       <c r="Q159" t="n">
-        <v>3.371648351648346</v>
+        <v>2.979999999999999</v>
       </c>
       <c r="R159" t="n">
         <v>0.25</v>
       </c>
       <c r="S159" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T159" t="inlineStr">
         <is>
@@ -27585,7 +27585,7 @@
         <v>0</v>
       </c>
       <c r="S160" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="T160" t="inlineStr">
         <is>
@@ -27656,7 +27656,7 @@
         <v>43456.62049768519</v>
       </c>
       <c r="AH160" t="n">
-        <v>4.962844630259907</v>
+        <v>4.897839799950911</v>
       </c>
       <c r="AI160" t="n">
         <v>0</v>
@@ -27755,7 +27755,7 @@
         <v>0.25</v>
       </c>
       <c r="S161" t="n">
-        <v>0.6600000000000001</v>
+        <v>6</v>
       </c>
       <c r="T161" t="inlineStr">
         <is>
@@ -28023,7 +28023,7 @@
         <v>0</v>
       </c>
       <c r="AQ162" t="n">
-        <v>2.903460327090944</v>
+        <v>2.870157652698332</v>
       </c>
       <c r="AR162" t="n">
         <v>1.414213562373095</v>
@@ -28193,7 +28193,7 @@
         <v>0</v>
       </c>
       <c r="AQ163" t="n">
-        <v>0.3492245082422</v>
+        <v>0.3980770808024077</v>
       </c>
       <c r="AR163" t="n">
         <v>1</v>
@@ -28202,7 +28202,7 @@
         <v>-0.9775626147275808</v>
       </c>
       <c r="AT163" t="n">
-        <v>-1.386434771566756</v>
+        <v>-1.067611178260432</v>
       </c>
     </row>
     <row r="164">
@@ -28216,7 +28216,7 @@
         <v>0</v>
       </c>
       <c r="D164" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -28235,7 +28235,7 @@
         <v>1</v>
       </c>
       <c r="I164" t="n">
-        <v>0.677</v>
+        <v>1</v>
       </c>
       <c r="J164" t="n">
         <v>1</v>
@@ -28265,7 +28265,7 @@
         <v>0.25</v>
       </c>
       <c r="S164" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="T164" t="inlineStr">
         <is>
@@ -28342,7 +28342,7 @@
         <v>0</v>
       </c>
       <c r="AJ164" t="n">
-        <v>0.5170064828410719</v>
+        <v>0.6931471805599453</v>
       </c>
       <c r="AK164" t="n">
         <v>3.931825632724326</v>
@@ -28366,7 +28366,7 @@
         <v>0.6182167368846151</v>
       </c>
       <c r="AR164" t="n">
-        <v>0.8228000972289685</v>
+        <v>1</v>
       </c>
       <c r="AS164" t="n">
         <v>-0.09056796595785398</v>
@@ -28506,7 +28506,7 @@
         <v>43415.5949537037</v>
       </c>
       <c r="AH165" t="n">
-        <v>4.912654885736052</v>
+        <v>4.897839799950911</v>
       </c>
       <c r="AI165" t="n">
         <v>0</v>
@@ -28861,7 +28861,7 @@
         <v>1.6094379124341</v>
       </c>
       <c r="AM167" t="n">
-        <v>2.70805020110221</v>
+        <v>2.564949357461537</v>
       </c>
       <c r="AN167" t="n">
         <v>10.81979828421029</v>
@@ -29186,7 +29186,7 @@
         <v>43471.29651620371</v>
       </c>
       <c r="AH169" t="n">
-        <v>4.990432586778736</v>
+        <v>4.897839799950911</v>
       </c>
       <c r="AI169" t="n">
         <v>0</v>
@@ -29213,7 +29213,7 @@
         <v>0</v>
       </c>
       <c r="AQ169" t="n">
-        <v>0.3189200420154253</v>
+        <v>0.3980770808024077</v>
       </c>
       <c r="AR169" t="n">
         <v>1</v>
@@ -29541,7 +29541,7 @@
         <v>1.945910149055313</v>
       </c>
       <c r="AM171" t="n">
-        <v>2.70805020110221</v>
+        <v>2.564949357461537</v>
       </c>
       <c r="AN171" t="n">
         <v>11.28979441357789</v>
@@ -29619,7 +29619,7 @@
         <v>54</v>
       </c>
       <c r="Q172" t="n">
-        <v>0.6944444444444444</v>
+        <v>0.8994612068965517</v>
       </c>
       <c r="R172" t="n">
         <v>0.25</v>
@@ -29723,7 +29723,7 @@
         <v>2</v>
       </c>
       <c r="AQ172" t="n">
-        <v>2.911284355548572</v>
+        <v>2.870157652698332</v>
       </c>
       <c r="AR172" t="n">
         <v>1</v>
@@ -29965,7 +29965,7 @@
         <v>0.5</v>
       </c>
       <c r="S174" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T174" t="inlineStr">
         <is>
@@ -30743,7 +30743,7 @@
         <v>0</v>
       </c>
       <c r="AQ178" t="n">
-        <v>0.3757008796881073</v>
+        <v>0.3980770808024077</v>
       </c>
       <c r="AR178" t="n">
         <v>1.414213562373095</v>
@@ -30886,7 +30886,7 @@
         <v>43472.57777777778</v>
       </c>
       <c r="AH179" t="n">
-        <v>3.714810443399589</v>
+        <v>4.23245935673567</v>
       </c>
       <c r="AI179" t="n">
         <v>0</v>
@@ -31247,13 +31247,13 @@
         <v>11.69525535506279</v>
       </c>
       <c r="AO181" t="n">
-        <v>14.5086582385241</v>
+        <v>14.31628645193719</v>
       </c>
       <c r="AP181" t="n">
         <v>2</v>
       </c>
       <c r="AQ181" t="n">
-        <v>3.509354993627202</v>
+        <v>2.870157652698332</v>
       </c>
       <c r="AR181" t="n">
         <v>1.414213562373095</v>
@@ -31417,7 +31417,7 @@
         <v>11.69525535506279</v>
       </c>
       <c r="AO182" t="n">
-        <v>12.41534077536593</v>
+        <v>12.76569129060437</v>
       </c>
       <c r="AP182" t="n">
         <v>2</v>
@@ -31587,13 +31587,13 @@
         <v>11.69525535506279</v>
       </c>
       <c r="AO183" t="n">
-        <v>12.42922019683638</v>
+        <v>12.76569129060437</v>
       </c>
       <c r="AP183" t="n">
         <v>0</v>
       </c>
       <c r="AQ183" t="n">
-        <v>0.391770934801162</v>
+        <v>0.3980770808024077</v>
       </c>
       <c r="AR183" t="n">
         <v>1.732050807568877</v>
@@ -31635,7 +31635,7 @@
         <v>1</v>
       </c>
       <c r="I184" t="n">
-        <v>0.677</v>
+        <v>1</v>
       </c>
       <c r="J184" t="n">
         <v>1</v>
@@ -31656,7 +31656,7 @@
         <v>3</v>
       </c>
       <c r="P184" t="n">
-        <v>60.33999999999997</v>
+        <v>58</v>
       </c>
       <c r="Q184" t="n">
         <v>2.421052631578947</v>
@@ -31742,7 +31742,7 @@
         <v>0</v>
       </c>
       <c r="AJ184" t="n">
-        <v>0.5170064828410719</v>
+        <v>0.6931471805599453</v>
       </c>
       <c r="AK184" t="n">
         <v>4.61512051684126</v>
@@ -31766,7 +31766,7 @@
         <v>2.735134410081278</v>
       </c>
       <c r="AR184" t="n">
-        <v>0.8228000972289685</v>
+        <v>1</v>
       </c>
       <c r="AS184" t="n">
         <v>0.1414900218948392</v>
@@ -31999,7 +31999,7 @@
         <v>53</v>
       </c>
       <c r="Q186" t="n">
-        <v>3.266666666666667</v>
+        <v>2.979999999999999</v>
       </c>
       <c r="R186" t="n">
         <v>0.5</v>
@@ -32685,7 +32685,7 @@
         <v>0.5</v>
       </c>
       <c r="S190" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="T190" t="inlineStr">
         <is>
@@ -33356,7 +33356,7 @@
         <v>3</v>
       </c>
       <c r="P194" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Q194" t="n">
         <v>2</v>
@@ -33457,13 +33457,13 @@
         <v>12.10071768541247</v>
       </c>
       <c r="AO194" t="n">
-        <v>12.67607939977103</v>
+        <v>12.76569129060437</v>
       </c>
       <c r="AP194" t="n">
         <v>2</v>
       </c>
       <c r="AQ194" t="n">
-        <v>0.3573225425015104</v>
+        <v>0.3980770808024077</v>
       </c>
       <c r="AR194" t="n">
         <v>1.414213562373095</v>
@@ -33526,7 +33526,7 @@
         <v>3</v>
       </c>
       <c r="P195" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q195" t="n">
         <v>1.772727272727273</v>
@@ -33656,7 +33656,7 @@
         <v>0</v>
       </c>
       <c r="D196" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -34206,10 +34206,10 @@
         <v>3</v>
       </c>
       <c r="P199" t="n">
-        <v>60.33999999999997</v>
+        <v>58</v>
       </c>
       <c r="Q199" t="n">
-        <v>3.0625</v>
+        <v>2.979999999999999</v>
       </c>
       <c r="R199" t="n">
         <v>0.25</v>
@@ -34286,13 +34286,13 @@
         <v>43412.3396875</v>
       </c>
       <c r="AH199" t="n">
-        <v>3.988984046564275</v>
+        <v>4.23245935673567</v>
       </c>
       <c r="AI199" t="n">
         <v>0</v>
       </c>
       <c r="AJ199" t="n">
-        <v>0.5170064828410719</v>
+        <v>0.6931471805599453</v>
       </c>
       <c r="AK199" t="n">
         <v>5.017279836814924</v>
@@ -34456,13 +34456,13 @@
         <v>43414.68344907407</v>
       </c>
       <c r="AH200" t="n">
-        <v>7.122464801919641</v>
+        <v>4.897839799950911</v>
       </c>
       <c r="AI200" t="n">
         <v>0</v>
       </c>
       <c r="AJ200" t="n">
-        <v>0.5170064828410719</v>
+        <v>0.6931471805599453</v>
       </c>
       <c r="AK200" t="n">
         <v>4.61512051684126</v>
@@ -34492,7 +34492,7 @@
         <v>0.2778970710793907</v>
       </c>
       <c r="AT200" t="n">
-        <v>-1.339177853439447</v>
+        <v>-1.067611178260432</v>
       </c>
     </row>
     <row r="201">
@@ -34506,7 +34506,7 @@
         <v>0</v>
       </c>
       <c r="D201" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -34525,7 +34525,7 @@
         <v>1</v>
       </c>
       <c r="I201" t="n">
-        <v>0.677</v>
+        <v>1</v>
       </c>
       <c r="J201" t="n">
         <v>1</v>
@@ -34546,7 +34546,7 @@
         <v>4</v>
       </c>
       <c r="P201" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Q201" t="n">
         <v>1.391304347826087</v>
@@ -34632,7 +34632,7 @@
         <v>0</v>
       </c>
       <c r="AJ201" t="n">
-        <v>0.5170064828410719</v>
+        <v>0.6931471805599453</v>
       </c>
       <c r="AK201" t="n">
         <v>4.61512051684126</v>
@@ -34656,7 +34656,7 @@
         <v>1.877597760018266</v>
       </c>
       <c r="AR201" t="n">
-        <v>0.8228000972289685</v>
+        <v>1</v>
       </c>
       <c r="AS201" t="n">
         <v>1.0245327994572</v>
@@ -35321,7 +35321,7 @@
         <v>1.791759469228055</v>
       </c>
       <c r="AM205" t="n">
-        <v>2.639057329615258</v>
+        <v>2.564949357461537</v>
       </c>
       <c r="AN205" t="n">
         <v>12.20607764551767</v>
@@ -35909,7 +35909,7 @@
         <v>48</v>
       </c>
       <c r="Q209" t="n">
-        <v>3.133333333333333</v>
+        <v>2.979999999999999</v>
       </c>
       <c r="R209" t="n">
         <v>0.25</v>
@@ -36716,7 +36716,7 @@
         <v>0</v>
       </c>
       <c r="D214" t="n">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -36747,7 +36747,7 @@
         <v>1</v>
       </c>
       <c r="M214" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N214" t="n">
         <v>4</v>
@@ -36863,7 +36863,7 @@
         <v>0</v>
       </c>
       <c r="AQ214" t="n">
-        <v>2.875200312436719</v>
+        <v>2.870157652698332</v>
       </c>
       <c r="AR214" t="n">
         <v>1.414213562373095</v>
@@ -37883,7 +37883,7 @@
         <v>2</v>
       </c>
       <c r="AQ220" t="n">
-        <v>0.3189200420154253</v>
+        <v>0.3980770808024077</v>
       </c>
       <c r="AR220" t="n">
         <v>1</v>
@@ -38026,7 +38026,7 @@
         <v>43428.29141203704</v>
       </c>
       <c r="AH221" t="n">
-        <v>3.714810443399589</v>
+        <v>4.23245935673567</v>
       </c>
       <c r="AI221" t="n">
         <v>0</v>
@@ -38286,10 +38286,10 @@
         <v>3</v>
       </c>
       <c r="P223" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q223" t="n">
-        <v>3.371648351648346</v>
+        <v>2.979999999999999</v>
       </c>
       <c r="R223" t="n">
         <v>0.75</v>
@@ -38551,7 +38551,7 @@
         <v>1.791759469228055</v>
       </c>
       <c r="AM224" t="n">
-        <v>2.70805020110221</v>
+        <v>2.564949357461537</v>
       </c>
       <c r="AN224" t="n">
         <v>12.42922019683638</v>
@@ -38903,7 +38903,7 @@
         <v>0</v>
       </c>
       <c r="AQ226" t="n">
-        <v>2.907939548846266</v>
+        <v>2.870157652698332</v>
       </c>
       <c r="AR226" t="n">
         <v>1.414213562373095</v>
@@ -38926,7 +38926,7 @@
         <v>0</v>
       </c>
       <c r="D227" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -39422,7 +39422,7 @@
         <v>0.001506306289517659</v>
       </c>
       <c r="AT229" t="n">
-        <v>-1.101871795475964</v>
+        <v>-1.067611178260432</v>
       </c>
     </row>
     <row r="230">
@@ -39436,7 +39436,7 @@
         <v>0</v>
       </c>
       <c r="D230" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -40165,7 +40165,7 @@
         <v>0.5</v>
       </c>
       <c r="S234" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="T234" t="inlineStr">
         <is>
@@ -40236,7 +40236,7 @@
         <v>43473.28554398148</v>
       </c>
       <c r="AH234" t="n">
-        <v>3.970291913552122</v>
+        <v>4.23245935673567</v>
       </c>
       <c r="AI234" t="n">
         <v>0</v>
@@ -40499,7 +40499,7 @@
         <v>53</v>
       </c>
       <c r="Q236" t="n">
-        <v>3</v>
+        <v>2.979999999999999</v>
       </c>
       <c r="R236" t="n">
         <v>0.75</v>
@@ -40626,7 +40626,7 @@
         <v>0</v>
       </c>
       <c r="D237" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -40916,7 +40916,7 @@
         <v>43454.68414351852</v>
       </c>
       <c r="AH238" t="n">
-        <v>4.969813299576001</v>
+        <v>4.897839799950911</v>
       </c>
       <c r="AI238" t="n">
         <v>0</v>
@@ -41136,7 +41136,7 @@
         <v>0</v>
       </c>
       <c r="D240" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -41176,7 +41176,7 @@
         <v>3</v>
       </c>
       <c r="P240" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q240" t="n">
         <v>1.863636363636364</v>
@@ -41262,7 +41262,7 @@
         <v>0</v>
       </c>
       <c r="AJ240" t="n">
-        <v>0.5170064828410719</v>
+        <v>0.6931471805599453</v>
       </c>
       <c r="AK240" t="n">
         <v>4.61512051684126</v>
@@ -41426,13 +41426,13 @@
         <v>43414.59118055556</v>
       </c>
       <c r="AH241" t="n">
-        <v>7.092573715974678</v>
+        <v>4.897839799950911</v>
       </c>
       <c r="AI241" t="n">
         <v>0</v>
       </c>
       <c r="AJ241" t="n">
-        <v>0.5170064828410719</v>
+        <v>0.6931471805599453</v>
       </c>
       <c r="AK241" t="n">
         <v>4.61512051684126</v>
@@ -41495,7 +41495,7 @@
         <v>1</v>
       </c>
       <c r="I242" t="n">
-        <v>0.677</v>
+        <v>1</v>
       </c>
       <c r="J242" t="n">
         <v>1</v>
@@ -41516,7 +41516,7 @@
         <v>4</v>
       </c>
       <c r="P242" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="Q242" t="n">
         <v>1.631578947368421</v>
@@ -41617,7 +41617,7 @@
         <v>12.61154108696612</v>
       </c>
       <c r="AO242" t="n">
-        <v>14.5086582385241</v>
+        <v>14.31628645193719</v>
       </c>
       <c r="AP242" t="n">
         <v>2</v>
@@ -41626,7 +41626,7 @@
         <v>0.676003306564684</v>
       </c>
       <c r="AR242" t="n">
-        <v>0.8228000972289685</v>
+        <v>1</v>
       </c>
       <c r="AS242" t="n">
         <v>0.7225050345983459</v>
@@ -41686,10 +41686,10 @@
         <v>4</v>
       </c>
       <c r="P243" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q243" t="n">
-        <v>0.8387096774193549</v>
+        <v>0.8994612068965517</v>
       </c>
       <c r="R243" t="n">
         <v>0.75</v>
@@ -41787,7 +41787,7 @@
         <v>12.61154108696612</v>
       </c>
       <c r="AO243" t="n">
-        <v>14.40329777842179</v>
+        <v>14.31628645193719</v>
       </c>
       <c r="AP243" t="n">
         <v>2</v>
@@ -42106,7 +42106,7 @@
         <v>43433.30201388889</v>
       </c>
       <c r="AH245" t="n">
-        <v>4.007333185232471</v>
+        <v>4.23245935673567</v>
       </c>
       <c r="AI245" t="n">
         <v>0</v>
@@ -42127,7 +42127,7 @@
         <v>12.61154108696612</v>
       </c>
       <c r="AO245" t="n">
-        <v>14.40329777842179</v>
+        <v>14.31628645193719</v>
       </c>
       <c r="AP245" t="n">
         <v>0</v>
@@ -42369,7 +42369,7 @@
         <v>46</v>
       </c>
       <c r="Q247" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8994612068965517</v>
       </c>
       <c r="R247" t="n">
         <v>0.75</v>
@@ -42706,7 +42706,7 @@
         <v>3</v>
       </c>
       <c r="P249" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q249" t="n">
         <v>2.578947368421053</v>
@@ -42786,7 +42786,7 @@
         <v>43415.31839120371</v>
       </c>
       <c r="AH249" t="n">
-        <v>7.122464801919641</v>
+        <v>4.897839799950911</v>
       </c>
       <c r="AI249" t="n">
         <v>0</v>
@@ -42822,7 +42822,7 @@
         <v>0.1767043868363914</v>
       </c>
       <c r="AT249" t="n">
-        <v>-1.162272465013724</v>
+        <v>-1.067611178260432</v>
       </c>
     </row>
     <row r="250">
@@ -43153,7 +43153,7 @@
         <v>2</v>
       </c>
       <c r="AQ251" t="n">
-        <v>0.3189200420154253</v>
+        <v>0.3980770808024077</v>
       </c>
       <c r="AR251" t="n">
         <v>1.414213562373095</v>
@@ -43559,7 +43559,7 @@
         <v>47</v>
       </c>
       <c r="Q254" t="n">
-        <v>0.6774193548387096</v>
+        <v>0.8994612068965517</v>
       </c>
       <c r="R254" t="n">
         <v>0.25</v>
@@ -43905,7 +43905,7 @@
         <v>0.75</v>
       </c>
       <c r="S256" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T256" t="inlineStr">
         <is>
@@ -44196,7 +44196,7 @@
         <v>0</v>
       </c>
       <c r="D258" t="n">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -44239,7 +44239,7 @@
         <v>50</v>
       </c>
       <c r="Q258" t="n">
-        <v>0.7058823529411765</v>
+        <v>0.8994612068965517</v>
       </c>
       <c r="R258" t="n">
         <v>0.5</v>
@@ -44337,7 +44337,7 @@
         <v>13.01700508396626</v>
       </c>
       <c r="AO258" t="n">
-        <v>14.40329777842179</v>
+        <v>14.31628645193719</v>
       </c>
       <c r="AP258" t="n">
         <v>2</v>
@@ -44513,7 +44513,7 @@
         <v>2</v>
       </c>
       <c r="AQ259" t="n">
-        <v>3.509354993627202</v>
+        <v>2.870157652698332</v>
       </c>
       <c r="AR259" t="n">
         <v>1.732050807568877</v>
@@ -44671,7 +44671,7 @@
         <v>1.791759469228055</v>
       </c>
       <c r="AM260" t="n">
-        <v>2.70805020110221</v>
+        <v>2.564949357461537</v>
       </c>
       <c r="AN260" t="n">
         <v>13.12236537740233</v>
@@ -44916,7 +44916,7 @@
         <v>3</v>
       </c>
       <c r="P262" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q262" t="n">
         <v>2.526315789473684</v>
@@ -45046,7 +45046,7 @@
         <v>1</v>
       </c>
       <c r="D263" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -45202,7 +45202,7 @@
         <v>0.7895241680226522</v>
       </c>
       <c r="AT263" t="n">
-        <v>1.24215712219905</v>
+        <v>1.136144008800468</v>
       </c>
     </row>
     <row r="264">
@@ -45363,7 +45363,7 @@
         <v>2</v>
       </c>
       <c r="AQ264" t="n">
-        <v>0.3768105557894013</v>
+        <v>0.3980770808024077</v>
       </c>
       <c r="AR264" t="n">
         <v>1.732050807568877</v>
@@ -45542,7 +45542,7 @@
         <v>0.8739874722154102</v>
       </c>
       <c r="AT265" t="n">
-        <v>1.322596814292072</v>
+        <v>1.136144008800468</v>
       </c>
     </row>
     <row r="266">
@@ -45605,7 +45605,7 @@
         <v>1</v>
       </c>
       <c r="S266" t="n">
-        <v>34.33999999999997</v>
+        <v>30</v>
       </c>
       <c r="T266" t="inlineStr">
         <is>
@@ -45685,7 +45685,7 @@
         <v>1.386294361119891</v>
       </c>
       <c r="AK266" t="n">
-        <v>6.90875477931522</v>
+        <v>6.398594934535208</v>
       </c>
       <c r="AL266" t="n">
         <v>2.19722457733622</v>
@@ -45694,10 +45694,10 @@
         <v>2.564949357461537</v>
       </c>
       <c r="AN266" t="n">
-        <v>13.45883704259595</v>
+        <v>13.30468660086356</v>
       </c>
       <c r="AO266" t="n">
-        <v>14.5086582385241</v>
+        <v>14.31628645193719</v>
       </c>
       <c r="AP266" t="n">
         <v>2</v>
@@ -45709,7 +45709,7 @@
         <v>2</v>
       </c>
       <c r="AS266" t="n">
-        <v>1.030581111831185</v>
+        <v>1.025823431465835</v>
       </c>
       <c r="AT266" t="n">
         <v>0.2021665100364722</v>
@@ -45852,7 +45852,7 @@
         <v>0</v>
       </c>
       <c r="AJ267" t="n">
-        <v>0.5170064828410719</v>
+        <v>0.6931471805599453</v>
       </c>
       <c r="AK267" t="n">
         <v>4.61512051684126</v>
@@ -45864,10 +45864,10 @@
         <v>0</v>
       </c>
       <c r="AN267" t="n">
-        <v>13.71015115341694</v>
+        <v>13.30468660086356</v>
       </c>
       <c r="AO267" t="n">
-        <v>12.61154108696612</v>
+        <v>12.76569129060437</v>
       </c>
       <c r="AP267" t="n">
         <v>2</v>
@@ -45879,10 +45879,10 @@
         <v>1.163615056623108</v>
       </c>
       <c r="AS267" t="n">
-        <v>1.432778152223154</v>
+        <v>1.025823431465835</v>
       </c>
       <c r="AT267" t="n">
-        <v>1.146509179953154</v>
+        <v>1.136144008800468</v>
       </c>
     </row>
     <row r="268">
@@ -45927,7 +45927,7 @@
         <v>1</v>
       </c>
       <c r="M268" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N268" t="n">
         <v>4</v>
@@ -46016,7 +46016,7 @@
         <v>43418.51855324074</v>
       </c>
       <c r="AH268" t="n">
-        <v>4.204692619390966</v>
+        <v>4.23245935673567</v>
       </c>
       <c r="AI268" t="n">
         <v>0</v>
@@ -46034,7 +46034,7 @@
         <v>1.6094379124341</v>
       </c>
       <c r="AN268" t="n">
-        <v>13.99783294809122</v>
+        <v>13.30468660086356</v>
       </c>
       <c r="AO268" t="n">
         <v>13.99783294809122</v>
@@ -46043,7 +46043,7 @@
         <v>2</v>
       </c>
       <c r="AQ268" t="n">
-        <v>3.509354993627202</v>
+        <v>2.870157652698332</v>
       </c>
       <c r="AR268" t="n">
         <v>1.732050807568877</v>

</xml_diff>